<commit_message>
Integrate new Alik'r weapons
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926F084E-0566-4E62-80AE-F3F7AB95C55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF589D1-E701-4DA1-A59D-26AFDE5E4441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="181">
   <si>
     <t>Primary</t>
   </si>
@@ -101,478 +101,487 @@
     <t>Orcish</t>
   </si>
   <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>SkyforgeSteel</t>
+  </si>
+  <si>
+    <t>Stalhrim</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>AncientNord</t>
+  </si>
+  <si>
+    <t>AncientNordHoned</t>
+  </si>
+  <si>
+    <t>Dragon Bone</t>
+  </si>
+  <si>
+    <t>Moonstone</t>
+  </si>
+  <si>
+    <t>Chaurus Chitin</t>
+  </si>
+  <si>
+    <t>Leather</t>
+  </si>
+  <si>
+    <t>Malachite</t>
+  </si>
+  <si>
+    <t>Orichalcum</t>
+  </si>
+  <si>
+    <t>Quicksilver</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Tanto</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>Shortsword</t>
+  </si>
+  <si>
+    <t>Wakizashi</t>
+  </si>
+  <si>
+    <t>WarAxe</t>
+  </si>
+  <si>
+    <t>Hatchet</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Maul</t>
+  </si>
+  <si>
+    <t>Greatsword</t>
+  </si>
+  <si>
+    <t>DaiKatana</t>
+  </si>
+  <si>
+    <t>Battleaxe</t>
+  </si>
+  <si>
+    <t>Warhammer</t>
+  </si>
+  <si>
+    <t>LongMace</t>
+  </si>
+  <si>
+    <t>Quarterstaff</t>
+  </si>
+  <si>
+    <t>Battlestaff</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
+  </si>
+  <si>
+    <t>Spectral</t>
+  </si>
+  <si>
+    <t>Ectoplasm</t>
+  </si>
+  <si>
+    <t>Corundum</t>
+  </si>
+  <si>
+    <t>Daedric</t>
+  </si>
+  <si>
+    <t>DawnguardImproved</t>
+  </si>
+  <si>
+    <t>Dwemer</t>
+  </si>
+  <si>
+    <t>DwemerImproved</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>BladeOfSacrifice</t>
+  </si>
+  <si>
+    <t>Bloodscythe</t>
+  </si>
+  <si>
+    <t>BloodskalBlade</t>
+  </si>
+  <si>
+    <t>ChampionsCudgel</t>
+  </si>
+  <si>
+    <t>Chillrend</t>
+  </si>
+  <si>
+    <t>Dawnbreaker</t>
+  </si>
+  <si>
+    <t>Dragonbane</t>
+  </si>
+  <si>
+    <t>DwarvenBlackBowOfFate</t>
+  </si>
+  <si>
+    <t>EbonyBlade</t>
+  </si>
+  <si>
+    <t>Ghostblade</t>
+  </si>
+  <si>
+    <t>GlassBowOfTheStagPrince</t>
+  </si>
+  <si>
+    <t>KahvozeinsFang</t>
+  </si>
+  <si>
+    <t>Keening</t>
+  </si>
+  <si>
+    <t>MehrunesRazor</t>
+  </si>
+  <si>
+    <t>Nettlebane</t>
+  </si>
+  <si>
+    <t>RedEaglesBane</t>
+  </si>
+  <si>
+    <t>RedEaglesFury</t>
+  </si>
+  <si>
+    <t>Soulrender</t>
+  </si>
+  <si>
+    <t>Stormfang</t>
+  </si>
+  <si>
+    <t>Volendrung</t>
+  </si>
+  <si>
+    <t>Windshear</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>RuefulAxe</t>
+  </si>
+  <si>
+    <t>Wuuthrad</t>
+  </si>
+  <si>
+    <t>Ebony_Battleaxe</t>
+  </si>
+  <si>
+    <t>Daedric_Dagger</t>
+  </si>
+  <si>
+    <t>Ebony_Dagger</t>
+  </si>
+  <si>
+    <t>Horksbane</t>
+  </si>
+  <si>
+    <t>RustyMace</t>
+  </si>
+  <si>
+    <t>Ebony_Greatsword</t>
+  </si>
+  <si>
+    <t>Daedric_Mace</t>
+  </si>
+  <si>
+    <t>Glass_Sword</t>
+  </si>
+  <si>
+    <t>Silver_Sword</t>
+  </si>
+  <si>
+    <t>Blades_Sword</t>
+  </si>
+  <si>
+    <t>Spectral_Sword</t>
+  </si>
+  <si>
+    <t>Daedric_Sword</t>
+  </si>
+  <si>
+    <t>Ebony_Sword</t>
+  </si>
+  <si>
+    <t>NordHero_Sword</t>
+  </si>
+  <si>
+    <t>Dawnguard_WarAxe</t>
+  </si>
+  <si>
+    <t>Orcish_Warhammer</t>
+  </si>
+  <si>
+    <t>Dawnguard_Warhammer</t>
+  </si>
+  <si>
+    <t>AetherialStaff</t>
+  </si>
+  <si>
+    <t>AncientDawnguardWarAxe</t>
+  </si>
+  <si>
+    <t>AncientDawnguardWarhammer</t>
+  </si>
+  <si>
+    <t>AurielsBow</t>
+  </si>
+  <si>
+    <t>AwakenedBladeOfWoe</t>
+  </si>
+  <si>
+    <t>BladeOfWoe</t>
+  </si>
+  <si>
+    <t>BrokenStaff</t>
+  </si>
+  <si>
+    <t>DragonPriestStaff</t>
+  </si>
+  <si>
+    <t>EyeOfMelka</t>
+  </si>
+  <si>
+    <t>GadnorsStaffOfCharming</t>
+  </si>
+  <si>
+    <t>GoraksTrollGuttingKnife</t>
+  </si>
+  <si>
+    <t>HalldirsStaff</t>
+  </si>
+  <si>
+    <t>HarkonsSword</t>
+  </si>
+  <si>
+    <t>HevnoraaksStaff</t>
+  </si>
+  <si>
+    <t>MaceOfMolagBal</t>
+  </si>
+  <si>
+    <t>MiraaksStaff</t>
+  </si>
+  <si>
+    <t>MiraaksSword</t>
+  </si>
+  <si>
+    <t>NightingaleBlade</t>
+  </si>
+  <si>
+    <t>NightingaleBow</t>
+  </si>
+  <si>
+    <t>RahgotsStaff</t>
+  </si>
+  <si>
+    <t>SanguineRose</t>
+  </si>
+  <si>
+    <t>SildsStaff</t>
+  </si>
+  <si>
+    <t>SkullOfCorruption</t>
+  </si>
+  <si>
+    <t>StaffOfArcaneAuthority</t>
+  </si>
+  <si>
+    <t>StaffOfHagsWrath</t>
+  </si>
+  <si>
+    <t>StaffOfJyrikGauldurson</t>
+  </si>
+  <si>
+    <t>StaffOfMagnus</t>
+  </si>
+  <si>
+    <t>StaffOfRuunvald</t>
+  </si>
+  <si>
+    <t>StaffOfTandil</t>
+  </si>
+  <si>
+    <t>TheLonghammer</t>
+  </si>
+  <si>
+    <t>Wabbajack</t>
+  </si>
+  <si>
+    <t>WabbajackDA15</t>
+  </si>
+  <si>
+    <t>Dwarven_Bow</t>
+  </si>
+  <si>
+    <t>Daedric_Warhammer</t>
+  </si>
+  <si>
+    <t>Dragonbone_Dagger</t>
+  </si>
+  <si>
+    <t>Forsworn_Sword</t>
+  </si>
+  <si>
+    <t>Ebony_Bow</t>
+  </si>
+  <si>
+    <t>Elven_Bow</t>
+  </si>
+  <si>
+    <t>Dwarven_Dagger</t>
+  </si>
+  <si>
+    <t>Silver_Battleaxe</t>
+  </si>
+  <si>
+    <t>Perk</t>
+  </si>
+  <si>
+    <t>Craftsmanship</t>
+  </si>
+  <si>
+    <t>Daedric Smithing</t>
+  </si>
+  <si>
+    <t>Draconic Blacksmithing</t>
+  </si>
+  <si>
+    <t>Dwarven Smithing</t>
+  </si>
+  <si>
+    <t>Ebony Smithing</t>
+  </si>
+  <si>
+    <t>Elven Smithing</t>
+  </si>
+  <si>
+    <t>Glass Smithing</t>
+  </si>
+  <si>
+    <t>Golden Smithing</t>
+  </si>
+  <si>
+    <t>Madness Smithing</t>
+  </si>
+  <si>
+    <t>Orcish Smithing</t>
+  </si>
+  <si>
+    <t>Stalhrim Smithing</t>
+  </si>
+  <si>
+    <t>Advanced Blacksmithing</t>
+  </si>
+  <si>
+    <t>Arcane Craftsmanship</t>
+  </si>
+  <si>
+    <t>Amber Smithing</t>
+  </si>
+  <si>
+    <t>Dark Smithing</t>
+  </si>
+  <si>
+    <t>Divine</t>
+  </si>
+  <si>
+    <t>Skyforge Smithing</t>
+  </si>
+  <si>
+    <t>Silver_Greatsword</t>
+  </si>
+  <si>
+    <t>Steel_Greatsword</t>
+  </si>
+  <si>
+    <t>Glass_Bow</t>
+  </si>
+  <si>
+    <t>Steel_Mace</t>
+  </si>
+  <si>
+    <t>Steel_Warhammer</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>BoundMystic</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Reach</t>
+  </si>
+  <si>
+    <t>Stagger</t>
+  </si>
+  <si>
+    <t>Alikr</t>
+  </si>
+  <si>
+    <t>Boneshaver</t>
+  </si>
+  <si>
+    <t>Alikr_Sword</t>
+  </si>
+  <si>
     <t>Redguard</t>
   </si>
   <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>SkyforgeSteel</t>
-  </si>
-  <si>
-    <t>Stalhrim</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>AncientNord</t>
-  </si>
-  <si>
-    <t>AncientNordHoned</t>
-  </si>
-  <si>
-    <t>Dragon Bone</t>
-  </si>
-  <si>
-    <t>Moonstone</t>
-  </si>
-  <si>
-    <t>Chaurus Chitin</t>
-  </si>
-  <si>
-    <t>Leather</t>
-  </si>
-  <si>
-    <t>Malachite</t>
-  </si>
-  <si>
-    <t>Orichalcum</t>
-  </si>
-  <si>
-    <t>Quicksilver</t>
-  </si>
-  <si>
-    <t>Dark</t>
-  </si>
-  <si>
-    <t>Golden</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>Dagger</t>
-  </si>
-  <si>
-    <t>Tanto</t>
-  </si>
-  <si>
-    <t>Sword</t>
-  </si>
-  <si>
-    <t>Katana</t>
-  </si>
-  <si>
-    <t>Shortsword</t>
-  </si>
-  <si>
-    <t>Wakizashi</t>
-  </si>
-  <si>
-    <t>WarAxe</t>
-  </si>
-  <si>
-    <t>Hatchet</t>
-  </si>
-  <si>
-    <t>Mace</t>
-  </si>
-  <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>Maul</t>
-  </si>
-  <si>
-    <t>Greatsword</t>
-  </si>
-  <si>
-    <t>DaiKatana</t>
-  </si>
-  <si>
-    <t>Battleaxe</t>
-  </si>
-  <si>
-    <t>Warhammer</t>
-  </si>
-  <si>
-    <t>LongMace</t>
-  </si>
-  <si>
-    <t>Quarterstaff</t>
-  </si>
-  <si>
-    <t>Battlestaff</t>
-  </si>
-  <si>
-    <t>Bow</t>
-  </si>
-  <si>
-    <t>Crossbow</t>
-  </si>
-  <si>
-    <t>Spectral</t>
-  </si>
-  <si>
-    <t>Ectoplasm</t>
-  </si>
-  <si>
-    <t>Corundum</t>
-  </si>
-  <si>
-    <t>Daedric</t>
-  </si>
-  <si>
-    <t>DawnguardImproved</t>
-  </si>
-  <si>
-    <t>Dwemer</t>
-  </si>
-  <si>
-    <t>DwemerImproved</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>BladeOfSacrifice</t>
-  </si>
-  <si>
-    <t>Bloodscythe</t>
-  </si>
-  <si>
-    <t>BloodskalBlade</t>
-  </si>
-  <si>
-    <t>ChampionsCudgel</t>
-  </si>
-  <si>
-    <t>Chillrend</t>
-  </si>
-  <si>
-    <t>Dawnbreaker</t>
-  </si>
-  <si>
-    <t>Dragonbane</t>
-  </si>
-  <si>
-    <t>DwarvenBlackBowOfFate</t>
-  </si>
-  <si>
-    <t>EbonyBlade</t>
-  </si>
-  <si>
-    <t>Ghostblade</t>
-  </si>
-  <si>
-    <t>GlassBowOfTheStagPrince</t>
-  </si>
-  <si>
-    <t>KahvozeinsFang</t>
-  </si>
-  <si>
-    <t>Keening</t>
-  </si>
-  <si>
-    <t>MehrunesRazor</t>
-  </si>
-  <si>
-    <t>Nettlebane</t>
-  </si>
-  <si>
-    <t>RedEaglesBane</t>
-  </si>
-  <si>
-    <t>RedEaglesFury</t>
-  </si>
-  <si>
-    <t>Soulrender</t>
-  </si>
-  <si>
-    <t>Stormfang</t>
-  </si>
-  <si>
-    <t>Volendrung</t>
-  </si>
-  <si>
-    <t>Windshear</t>
-  </si>
-  <si>
-    <t>Zephyr</t>
-  </si>
-  <si>
-    <t>RuefulAxe</t>
-  </si>
-  <si>
-    <t>Wuuthrad</t>
-  </si>
-  <si>
-    <t>Ebony_Battleaxe</t>
-  </si>
-  <si>
-    <t>Daedric_Dagger</t>
-  </si>
-  <si>
-    <t>Ebony_Dagger</t>
-  </si>
-  <si>
-    <t>Horksbane</t>
-  </si>
-  <si>
-    <t>RustyMace</t>
-  </si>
-  <si>
-    <t>Ebony_Greatsword</t>
-  </si>
-  <si>
-    <t>Daedric_Mace</t>
-  </si>
-  <si>
-    <t>Glass_Sword</t>
-  </si>
-  <si>
-    <t>Silver_Sword</t>
-  </si>
-  <si>
-    <t>Blades_Sword</t>
-  </si>
-  <si>
-    <t>Spectral_Sword</t>
-  </si>
-  <si>
-    <t>Daedric_Sword</t>
-  </si>
-  <si>
-    <t>Ebony_Sword</t>
-  </si>
-  <si>
-    <t>NordHero_Sword</t>
-  </si>
-  <si>
     <t>Redguard_Sword</t>
-  </si>
-  <si>
-    <t>Dawnguard_WarAxe</t>
-  </si>
-  <si>
-    <t>Orcish_Warhammer</t>
-  </si>
-  <si>
-    <t>Dawnguard_Warhammer</t>
-  </si>
-  <si>
-    <t>AetherialStaff</t>
-  </si>
-  <si>
-    <t>AncientDawnguardWarAxe</t>
-  </si>
-  <si>
-    <t>AncientDawnguardWarhammer</t>
-  </si>
-  <si>
-    <t>AurielsBow</t>
-  </si>
-  <si>
-    <t>AwakenedBladeOfWoe</t>
-  </si>
-  <si>
-    <t>BladeOfWoe</t>
-  </si>
-  <si>
-    <t>BrokenStaff</t>
-  </si>
-  <si>
-    <t>DragonPriestStaff</t>
-  </si>
-  <si>
-    <t>EyeOfMelka</t>
-  </si>
-  <si>
-    <t>GadnorsStaffOfCharming</t>
-  </si>
-  <si>
-    <t>GoraksTrollGuttingKnife</t>
-  </si>
-  <si>
-    <t>HalldirsStaff</t>
-  </si>
-  <si>
-    <t>HarkonsSword</t>
-  </si>
-  <si>
-    <t>HevnoraaksStaff</t>
-  </si>
-  <si>
-    <t>MaceOfMolagBal</t>
-  </si>
-  <si>
-    <t>MiraaksStaff</t>
-  </si>
-  <si>
-    <t>MiraaksSword</t>
-  </si>
-  <si>
-    <t>NightingaleBlade</t>
-  </si>
-  <si>
-    <t>NightingaleBow</t>
-  </si>
-  <si>
-    <t>RahgotsStaff</t>
-  </si>
-  <si>
-    <t>SanguineRose</t>
-  </si>
-  <si>
-    <t>SildsStaff</t>
-  </si>
-  <si>
-    <t>SkullOfCorruption</t>
-  </si>
-  <si>
-    <t>StaffOfArcaneAuthority</t>
-  </si>
-  <si>
-    <t>StaffOfHagsWrath</t>
-  </si>
-  <si>
-    <t>StaffOfJyrikGauldurson</t>
-  </si>
-  <si>
-    <t>StaffOfMagnus</t>
-  </si>
-  <si>
-    <t>StaffOfRuunvald</t>
-  </si>
-  <si>
-    <t>StaffOfTandil</t>
-  </si>
-  <si>
-    <t>TheLonghammer</t>
-  </si>
-  <si>
-    <t>Wabbajack</t>
-  </si>
-  <si>
-    <t>WabbajackDA15</t>
-  </si>
-  <si>
-    <t>Dwarven_Bow</t>
-  </si>
-  <si>
-    <t>Daedric_Warhammer</t>
-  </si>
-  <si>
-    <t>Dragonbone_Dagger</t>
-  </si>
-  <si>
-    <t>Forsworn_Sword</t>
-  </si>
-  <si>
-    <t>Ebony_Bow</t>
-  </si>
-  <si>
-    <t>Elven_Bow</t>
-  </si>
-  <si>
-    <t>Dwarven_Dagger</t>
-  </si>
-  <si>
-    <t>Silver_Battleaxe</t>
-  </si>
-  <si>
-    <t>Perk</t>
-  </si>
-  <si>
-    <t>Craftsmanship</t>
-  </si>
-  <si>
-    <t>Daedric Smithing</t>
-  </si>
-  <si>
-    <t>Draconic Blacksmithing</t>
-  </si>
-  <si>
-    <t>Dwarven Smithing</t>
-  </si>
-  <si>
-    <t>Ebony Smithing</t>
-  </si>
-  <si>
-    <t>Elven Smithing</t>
-  </si>
-  <si>
-    <t>Glass Smithing</t>
-  </si>
-  <si>
-    <t>Golden Smithing</t>
-  </si>
-  <si>
-    <t>Madness Smithing</t>
-  </si>
-  <si>
-    <t>Orcish Smithing</t>
-  </si>
-  <si>
-    <t>Stalhrim Smithing</t>
-  </si>
-  <si>
-    <t>Advanced Blacksmithing</t>
-  </si>
-  <si>
-    <t>Arcane Craftsmanship</t>
-  </si>
-  <si>
-    <t>Amber Smithing</t>
-  </si>
-  <si>
-    <t>Dark Smithing</t>
-  </si>
-  <si>
-    <t>Divine</t>
-  </si>
-  <si>
-    <t>Skyforge Smithing</t>
-  </si>
-  <si>
-    <t>Silver_Greatsword</t>
-  </si>
-  <si>
-    <t>Steel_Greatsword</t>
-  </si>
-  <si>
-    <t>Glass_Bow</t>
-  </si>
-  <si>
-    <t>Steel_Mace</t>
-  </si>
-  <si>
-    <t>Steel_Warhammer</t>
-  </si>
-  <si>
-    <t>Bound</t>
-  </si>
-  <si>
-    <t>BoundMystic</t>
-  </si>
-  <si>
-    <t>Damage</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Reach</t>
-  </si>
-  <si>
-    <t>Stagger</t>
   </si>
 </sst>
 </file>
@@ -925,9 +934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -941,13 +952,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -959,243 +970,249 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1204,12 +1221,12 @@
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1218,161 +1235,152 @@
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D18">
-        <v>0.25</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="C21">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D21">
-        <v>25</v>
-      </c>
-      <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
+        <v>0.2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1380,129 +1388,129 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" s="1">
-        <v>1.3333333333333333</v>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H23" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
         <v>15</v>
       </c>
-      <c r="B24">
-        <v>-1</v>
-      </c>
-      <c r="C24">
-        <v>-1</v>
-      </c>
-      <c r="D24">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
       <c r="H24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D25">
-        <v>40</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" t="s">
-        <v>15</v>
+      <c r="G28" t="s">
+        <v>33</v>
       </c>
       <c r="H28" t="s">
         <v>158</v>
@@ -1510,27 +1518,30 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="G29" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1539,70 +1550,70 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B33">
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>40</v>
-      </c>
-      <c r="E33" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
       </c>
       <c r="H33" t="s">
         <v>159</v>
@@ -1610,45 +1621,65 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H34" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
         <v>-6</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>-7</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>0.25</v>
       </c>
-      <c r="E35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" t="s">
-        <v>149</v>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1672,27 +1703,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>175</v>
-      </c>
-      <c r="F1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1715,7 +1746,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1738,7 +1769,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1761,7 +1792,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -1784,7 +1815,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1807,7 +1838,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1830,7 +1861,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1853,7 +1884,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -1876,7 +1907,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -1899,7 +1930,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -1922,7 +1953,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -1945,7 +1976,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -1968,7 +1999,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1991,7 +2022,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -2014,7 +2045,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -2037,7 +2068,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -2060,7 +2091,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -2083,7 +2114,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -2133,12 +2164,12 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2152,7 +2183,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2166,7 +2197,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2180,7 +2211,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -2194,7 +2225,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2208,7 +2239,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2222,7 +2253,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -2236,7 +2267,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2250,7 +2281,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -2264,7 +2295,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2278,7 +2309,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2292,7 +2323,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -2306,7 +2337,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2320,7 +2351,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -2334,7 +2365,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2348,7 +2379,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -2362,7 +2393,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2376,7 +2407,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2390,7 +2421,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2404,7 +2435,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -2423,10 +2454,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,41 +2469,41 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>173</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>174</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>175</v>
       </c>
-      <c r="G1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" t="s">
-        <v>177</v>
-      </c>
       <c r="I1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2486,10 +2517,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2503,10 +2534,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -2514,10 +2545,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2534,10 +2565,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -2545,10 +2576,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2562,10 +2593,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -2573,10 +2604,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -2584,35 +2615,29 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11">
+        <v>5000</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-      <c r="E13">
-        <v>5000</v>
+        <v>168</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -2620,104 +2645,113 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
       </c>
       <c r="E14">
-        <v>80000</v>
+        <v>5000</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>5000</v>
+        <v>80000</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>5000</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>140</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18">
-        <v>-3</v>
-      </c>
-      <c r="E18">
-        <v>80000</v>
+        <v>138</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19">
+        <v>-3</v>
+      </c>
+      <c r="E19">
+        <v>80000</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21">
-        <v>5000</v>
-      </c>
-      <c r="I21" t="b">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>99</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
@@ -2725,19 +2759,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <v>1000</v>
+        <v>166</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -2745,60 +2770,66 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="B24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>1000</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>-8</v>
-      </c>
-      <c r="E25">
-        <v>5000</v>
-      </c>
-      <c r="F25">
-        <v>-0.125</v>
-      </c>
-      <c r="G25">
-        <v>0.05</v>
-      </c>
-      <c r="I25" t="b">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>-8</v>
+      </c>
+      <c r="E26">
+        <v>5000</v>
+      </c>
+      <c r="F26">
+        <v>-0.125</v>
+      </c>
+      <c r="G26">
+        <v>0.05</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" t="s">
-        <v>169</v>
-      </c>
-      <c r="I27" t="b">
-        <v>0</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
-      </c>
-      <c r="E28">
-        <v>5000</v>
+        <v>167</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -2806,33 +2837,30 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>2.5</v>
+        <v>140</v>
       </c>
       <c r="E29">
-        <v>80000</v>
+        <v>5000</v>
       </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>144</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E30">
         <v>80000</v>
@@ -2843,10 +2871,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
       </c>
       <c r="E31">
         <v>80000</v>
@@ -2857,60 +2888,63 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32">
+        <v>80000</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>-4</v>
+        <v>91</v>
       </c>
       <c r="E35">
         <v>5000</v>
       </c>
       <c r="I35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>101</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>-4</v>
+      </c>
+      <c r="E36">
+        <v>5000</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -2918,38 +2952,29 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38">
-        <v>5000</v>
-      </c>
-      <c r="F38">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G38">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I38" t="b">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39">
-        <v>-3</v>
+        <v>102</v>
+      </c>
+      <c r="E39">
+        <v>5000</v>
       </c>
       <c r="F39">
         <v>7.4999999999999997E-2</v>
@@ -2963,108 +2988,111 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="C40">
-        <v>7</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40">
-        <v>80000</v>
+        <v>-3</v>
+      </c>
+      <c r="F40">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G40">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>80000</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" t="s">
-        <v>102</v>
-      </c>
-      <c r="I45" t="b">
-        <v>0</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>82</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" t="s">
-        <v>167</v>
-      </c>
-      <c r="I52" t="b">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
-      </c>
-      <c r="D53">
-        <v>-9</v>
-      </c>
-      <c r="F53">
-        <v>0.2</v>
+        <v>165</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
@@ -3072,54 +3100,54 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="D54">
-        <v>5</v>
-      </c>
-      <c r="E54">
-        <v>80000</v>
+        <v>-9</v>
+      </c>
+      <c r="F54">
+        <v>0.2</v>
       </c>
       <c r="I54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>84</v>
+      </c>
+      <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>80000</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" t="s">
-        <v>104</v>
-      </c>
-      <c r="I57" t="b">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="E58">
-        <v>80000</v>
+        <v>180</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
@@ -3127,12 +3155,29 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>89</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>80000</v>
       </c>
       <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="I60" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Swap the stats of Dwarven and Orcish weapons
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAE34CC-E7F6-4BC7-9578-7F5A53FCBC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF13D69-44BD-425A-B6D3-8F5808FCBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,13 +1203,13 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
         <v>4</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1492,13 +1492,13 @@
         <v>18</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
         <v>31</v>
@@ -2453,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,10 +2854,10 @@
         <v>143</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="E30">
         <v>80000</v>

</xml_diff>

<commit_message>
Restore material bonus of Dawnguard weapons
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF13D69-44BD-425A-B6D3-8F5808FCBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2100D8-6ED0-4370-B3A1-5D67EDCFD723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,10 +1137,10 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -2453,7 +2453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix weight of tantos
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD40A25F-89FD-412B-80C8-448B450B453F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF3863-22C7-48B8-A8B0-D45520FB6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="244">
   <si>
     <t>Primary</t>
   </si>
@@ -1908,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7180504A-6B28-41F6-B85F-D857A0714427}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,7 +1919,7 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>157</v>
       </c>
@@ -1938,8 +1938,11 @@
       <c r="G1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1961,8 +1964,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1984,8 +1990,11 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2007,8 +2016,11 @@
       <c r="G5">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2030,8 +2042,11 @@
       <c r="G6">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2053,8 +2068,11 @@
       <c r="G7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2076,8 +2094,11 @@
       <c r="G8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2099,8 +2120,11 @@
       <c r="G10">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2122,8 +2146,11 @@
       <c r="G11">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2145,8 +2172,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2168,8 +2198,11 @@
       <c r="G14">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2191,8 +2224,11 @@
       <c r="G15">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2214,8 +2250,11 @@
       <c r="G17">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2237,8 +2276,11 @@
       <c r="G18">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2260,8 +2302,11 @@
       <c r="G20">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2283,8 +2328,11 @@
       <c r="G22">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2306,8 +2354,11 @@
       <c r="G23">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2329,8 +2380,11 @@
       <c r="G25">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2352,9 +2406,13 @@
       <c r="G26">
         <v>1.05</v>
       </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3708,7 +3766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F89DD17-A789-4A9A-885F-8377FED7E813}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tweaks stats of battlestaff and quarterstaff
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF3863-22C7-48B8-A8B0-D45520FB6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC114F-C7BF-4CA3-B81B-C1B255EECC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
@@ -1911,7 +1911,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,7 +2363,7 @@
         <v>41</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -2378,7 +2378,7 @@
         <v>1.3</v>
       </c>
       <c r="G25">
-        <v>1.05</v>
+        <v>1.2</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>10</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>80</v>

</xml_diff>

<commit_message>
Run all patcher scripts again
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226894CE-7DF5-4D47-966B-D3738D5A40F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1689537A-88B1-4C26-9C3A-BC491E569C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="302">
   <si>
     <t>Primary</t>
   </si>
@@ -720,9 +720,6 @@
     <t>Elven_Dagger</t>
   </si>
   <si>
-    <t>BowOfTheHunt</t>
-  </si>
-  <si>
     <t>BriarheartGeis</t>
   </si>
   <si>
@@ -940,6 +937,15 @@
   </si>
   <si>
     <t>Ebony_Katana</t>
+  </si>
+  <si>
+    <t>BowOfTheHawk</t>
+  </si>
+  <si>
+    <t>Quicksilver_Bow</t>
+  </si>
+  <si>
+    <t>Silver_Battleaxe</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3060,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,21 +3324,21 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>299</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>300</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" t="s">
         <v>227</v>
-      </c>
-      <c r="B21" t="s">
-        <v>228</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
@@ -3415,7 +3421,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
         <v>219</v>
@@ -3429,7 +3435,7 @@
         <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
@@ -3440,7 +3446,7 @@
         <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D30">
         <v>-3</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>74</v>
@@ -3481,7 +3487,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" t="s">
         <v>97</v>
@@ -3492,10 +3498,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>231</v>
+      </c>
+      <c r="B35" t="s">
         <v>232</v>
-      </c>
-      <c r="B35" t="s">
-        <v>233</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -3508,10 +3514,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" t="s">
         <v>234</v>
-      </c>
-      <c r="B37" t="s">
-        <v>235</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -3519,10 +3525,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" t="s">
         <v>236</v>
-      </c>
-      <c r="B38" t="s">
-        <v>237</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
@@ -3530,10 +3536,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" t="s">
         <v>238</v>
-      </c>
-      <c r="B39" t="s">
-        <v>239</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
@@ -3541,10 +3547,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" t="s">
         <v>240</v>
-      </c>
-      <c r="B40" t="s">
-        <v>241</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -3597,10 +3603,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
@@ -3613,10 +3619,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -3624,10 +3630,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -3635,7 +3641,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B48" t="s">
         <v>187</v>
@@ -3651,7 +3657,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B50" t="s">
         <v>191</v>
@@ -3707,7 +3713,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B54" t="s">
         <v>121</v>
@@ -3727,7 +3733,7 @@
         <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D55">
         <v>4</v>
@@ -3780,7 +3786,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
         <v>196</v>
@@ -3822,10 +3828,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>247</v>
+      </c>
+      <c r="B62" t="s">
         <v>248</v>
-      </c>
-      <c r="B62" t="s">
-        <v>249</v>
       </c>
       <c r="I62" t="b">
         <v>1</v>
@@ -3833,10 +3839,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B63" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I63" t="b">
         <v>0</v>
@@ -3844,7 +3850,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64" t="s">
         <v>225</v>
@@ -3855,10 +3861,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" t="s">
         <v>252</v>
-      </c>
-      <c r="B65" t="s">
-        <v>253</v>
       </c>
       <c r="I65" t="b">
         <v>0</v>
@@ -3866,7 +3872,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B66" t="s">
         <v>191</v>
@@ -3880,15 +3886,15 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E68">
         <v>5000</v>
@@ -3902,10 +3908,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F69">
         <v>7.4999999999999997E-2</v>
@@ -3916,13 +3922,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B70" t="s">
-        <v>285</v>
-      </c>
-      <c r="D70">
-        <v>-5</v>
+        <v>301</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
       </c>
       <c r="E70">
         <v>80000</v>
@@ -3933,7 +3939,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B71" t="s">
         <v>222</v>
@@ -3944,20 +3950,20 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>261</v>
+      </c>
+      <c r="B74" t="s">
         <v>262</v>
-      </c>
-      <c r="B74" t="s">
-        <v>263</v>
       </c>
       <c r="I74" t="b">
         <v>0</v>
@@ -3965,17 +3971,17 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B77" t="s">
         <v>73</v>
@@ -3986,40 +3992,40 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I84" t="b">
         <v>0</v>
@@ -4027,7 +4033,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B85" t="s">
         <v>194</v>
@@ -4041,10 +4047,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B86" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I86" t="b">
         <v>0</v>
@@ -4052,10 +4058,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B87" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I87" t="b">
         <v>0</v>
@@ -4063,7 +4069,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B88" t="s">
         <v>121</v>
@@ -4074,7 +4080,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B89" t="s">
         <v>222</v>
@@ -4085,10 +4091,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D90">
         <v>7</v>
@@ -4102,20 +4108,20 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>281</v>
+      </c>
+      <c r="B93" t="s">
         <v>282</v>
-      </c>
-      <c r="B93" t="s">
-        <v>283</v>
       </c>
       <c r="I93" t="b">
         <v>0</v>
@@ -4123,10 +4129,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I94" t="b">
         <v>0</v>
@@ -4134,10 +4140,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>283</v>
+      </c>
+      <c r="B95" t="s">
         <v>284</v>
-      </c>
-      <c r="B95" t="s">
-        <v>285</v>
       </c>
       <c r="E95">
         <v>50000</v>
@@ -4148,7 +4154,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B96" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Soulreaping weapons cannot be disenchanted
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1689537A-88B1-4C26-9C3A-BC491E569C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C187DA60-CB3C-45B0-AF4D-8BEC55B9A2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="303">
   <si>
     <t>Primary</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>Silver_Battleaxe</t>
+  </si>
+  <si>
+    <t>Soulreaping</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,93 +2084,116 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="D34">
-        <v>1</v>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G34" t="s">
-        <v>46</v>
+        <v>138</v>
+      </c>
+      <c r="H34" t="s">
+        <v>138</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>40</v>
-      </c>
-      <c r="E35" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" t="s">
-        <v>138</v>
-      </c>
-      <c r="H35" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>46</v>
       </c>
       <c r="I35" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
         <v>138</v>
       </c>
-      <c r="F36" t="s">
-        <v>143</v>
-      </c>
       <c r="H36" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>-6</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>-7</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>0.25</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>150</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>212</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I38" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3066,7 +3092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Soulreaping weapons cannot be disenchanted (#481)
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Weapon.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Weapon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1689537A-88B1-4C26-9C3A-BC491E569C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C187DA60-CB3C-45B0-AF4D-8BEC55B9A2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C480242-CFA6-464E-B2D0-26CF905FE2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="303">
   <si>
     <t>Primary</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>Silver_Battleaxe</t>
+  </si>
+  <si>
+    <t>Soulreaping</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DAB44D-10D6-48D9-84AA-13B1D653DD7B}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,93 +2084,116 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="D34">
-        <v>1</v>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G34" t="s">
-        <v>46</v>
+        <v>138</v>
+      </c>
+      <c r="H34" t="s">
+        <v>138</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>40</v>
-      </c>
-      <c r="E35" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" t="s">
-        <v>138</v>
-      </c>
-      <c r="H35" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>46</v>
       </c>
       <c r="I35" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
         <v>138</v>
       </c>
-      <c r="F36" t="s">
-        <v>143</v>
-      </c>
       <c r="H36" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>-6</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>-7</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>0.25</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>150</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>212</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I38" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3066,7 +3092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E600040-C4D1-44DA-89A7-D165F82BA4A4}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>

</xml_diff>